<commit_message>
Programs till Oct 13th
</commit_message>
<xml_diff>
--- a/HTML components.xlsx
+++ b/HTML components.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\006LiveTechWS\SeleniumSeasons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\005LiveTechWS\SeleniumSeasons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A27DB5AE-36DC-4616-8C7D-7C7D29BD15DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A002674-F1E4-4ADE-AA8E-F41B39B8EF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{40837B89-5355-4658-BD9D-8F1DCD533F26}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>HTML Component/
 WebElement</t>
@@ -59,6 +59,24 @@
   </si>
   <si>
     <t>id,name,class etc</t>
+  </si>
+  <si>
+    <t>dropdown</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>items in drop</t>
+  </si>
+  <si>
+    <t>option</t>
+  </si>
+  <si>
+    <t>value</t>
   </si>
 </sst>
 </file>
@@ -455,7 +473,7 @@
   <dimension ref="E3:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.3"/>
@@ -497,16 +515,32 @@
       </c>
     </row>
     <row r="5" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="5:8" x14ac:dyDescent="0.3">
       <c r="E7" s="2"/>

</xml_diff>